<commit_message>
updated stats & stuff
</commit_message>
<xml_diff>
--- a/HypothesisTesting.xlsx
+++ b/HypothesisTesting.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="420" windowWidth="21795" windowHeight="8985"/>
+    <workbookView xWindow="480" yWindow="420" windowWidth="7110" windowHeight="8985"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1 (2)" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="38">
   <si>
     <t>count</t>
   </si>
@@ -95,13 +96,66 @@
   <si>
     <t>g</t>
   </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>Q8</t>
+  </si>
+  <si>
+    <t>Q9</t>
+  </si>
+  <si>
+    <t>Q10</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>skew</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="4">
+    <numFmt numFmtId="192" formatCode="0.0000"/>
+    <numFmt numFmtId="194" formatCode="0.000000"/>
+    <numFmt numFmtId="195" formatCode="0.0000000"/>
+    <numFmt numFmtId="203" formatCode="0.000000000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -135,12 +189,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="192" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="194" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="195" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="203" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -174,9 +238,9 @@
       <sheetName val="Ken Tau Table"/>
       <sheetName val="Durbin Table"/>
       <sheetName val="Dunnett Table"/>
-      <sheetName val="RealStats-2010"/>
     </sheetNames>
     <definedNames>
+      <definedName name="SignTest"/>
       <definedName name="T_DIST"/>
     </definedNames>
     <sheetDataSet>
@@ -195,7 +259,6 @@
       <sheetData sheetId="12"/>
       <sheetData sheetId="13"/>
       <sheetData sheetId="14"/>
-      <sheetData sheetId="15" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -488,10 +551,3014 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AE70"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" customWidth="1"/>
+    <col min="20" max="20" width="15" customWidth="1"/>
+    <col min="25" max="25" width="13.28515625" customWidth="1"/>
+    <col min="30" max="30" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <f>COUNT(A2:A17)</f>
+        <v>16</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <f>COUNT(G2:G17)</f>
+        <v>16</v>
+      </c>
+      <c r="L2" s="1">
+        <v>2</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <f>COUNT(L2:L17)</f>
+        <v>15</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>1</v>
+      </c>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <f>COUNT(Q2:Q17)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <f>AVERAGE(A2:A17)</f>
+        <v>3.1875</v>
+      </c>
+      <c r="E3" s="1">
+        <f>MEDIAN(A2:A17)</f>
+        <v>3</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <f>AVERAGE(G2:G17)</f>
+        <v>3.125</v>
+      </c>
+      <c r="K3" s="1">
+        <f>MEDIAN(G2:G17)</f>
+        <v>3.5</v>
+      </c>
+      <c r="L3" s="1">
+        <v>2</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1">
+        <f>AVERAGE(L2:L17)</f>
+        <v>3.5333333333333332</v>
+      </c>
+      <c r="P3" s="1">
+        <f>MEDIAN(L2:L17)</f>
+        <v>4</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>1</v>
+      </c>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1">
+        <f>AVERAGE(Q2:Q17)</f>
+        <v>2.625</v>
+      </c>
+      <c r="U3" s="1">
+        <f>MEDIAN(Q2:Q17)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <f>_xlfn.STDEV.S(A2:A17)</f>
+        <v>1.1086778913041726</v>
+      </c>
+      <c r="E4" s="1">
+        <f>_xlfn.MODE.SNGL(A2:A17)</f>
+        <v>3</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
+        <v>2</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="1">
+        <f>_xlfn.STDEV.S(G2:G17)</f>
+        <v>1.0878112581387147</v>
+      </c>
+      <c r="K4" s="1">
+        <f>_xlfn.MODE.SNGL(G2:G17)</f>
+        <v>4</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O4" s="1">
+        <f>_xlfn.STDEV.S(L2:L17)</f>
+        <v>1.0600988273786189</v>
+      </c>
+      <c r="P4" s="1">
+        <f>_xlfn.MODE.SNGL(L2:L17)</f>
+        <v>4</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>2</v>
+      </c>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T4" s="1">
+        <f>_xlfn.STDEV.S(Q2:Q17)</f>
+        <v>0.9574271077563381</v>
+      </c>
+      <c r="U4" s="1">
+        <f>_xlfn.MODE.SNGL(Q2:Q17)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <f>D4/SQRT(D2)</f>
+        <v>0.27716947282604315</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" s="1">
+        <f>J4/SQRT(J2)</f>
+        <v>0.27195281453467868</v>
+      </c>
+      <c r="L5" s="1">
+        <v>3</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="1">
+        <f>O4/SQRT(O2)</f>
+        <v>0.27371634025142683</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>2</v>
+      </c>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T5" s="1">
+        <f>T4/SQRT(T2)</f>
+        <v>0.23935677693908453</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="L6" s="1">
+        <v>3</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="Q6" s="1">
+        <v>2</v>
+      </c>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+    </row>
+    <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="1">
+        <v>3</v>
+      </c>
+      <c r="L7" s="1">
+        <v>3</v>
+      </c>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>2</v>
+      </c>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1">
+        <v>3</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="L8" s="1">
+        <v>3</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O8" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>2</v>
+      </c>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1">
+        <v>3</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="1">
+        <v>2</v>
+      </c>
+      <c r="L9" s="1">
+        <v>4</v>
+      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O9" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>3</v>
+      </c>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>3</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1">
+        <f>D2-1</f>
+        <v>15</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1">
+        <v>4</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10" s="1">
+        <f>J2-1</f>
+        <v>15</v>
+      </c>
+      <c r="L10" s="1">
+        <v>4</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O10" s="1">
+        <f>O2-1</f>
+        <v>14</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>3</v>
+      </c>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T10" s="1">
+        <f>T2-1</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1">
+        <f>(D3-D7)/D5</f>
+        <v>0.67648142520254595</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1">
+        <v>4</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="1">
+        <f>(J3-J7)/J5</f>
+        <v>0.4596385597769217</v>
+      </c>
+      <c r="L11" s="1">
+        <v>4</v>
+      </c>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O11" s="1">
+        <f>(O3-O7)/O5</f>
+        <v>1.9484892017898192</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>3</v>
+      </c>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T11" s="1">
+        <f>ABS(T3-T7)/T5</f>
+        <v>1.5666989036012806</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <f>_xlfn.T.DIST.2T(D11,D10)</f>
+        <v>0.50903274081690952</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1">
+        <v>4</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12">
+        <f>_xlfn.T.DIST.RT(J11,J10)</f>
+        <v>0.32618352097097225</v>
+      </c>
+      <c r="L12" s="1">
+        <v>4</v>
+      </c>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12">
+        <f>_xlfn.T.DIST.2T(O11,O10)</f>
+        <v>7.1688101302534835E-2</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>3</v>
+      </c>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T12">
+        <f>_xlfn.T.DIST.2T(T11,T10)</f>
+        <v>0.13803484396804874</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1" t="str">
+        <f>IF(D12&lt;D8,"yes","no")</f>
+        <v>no</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1" t="str">
+        <f>IF(J12&lt;J8,"yes","no")</f>
+        <v>no</v>
+      </c>
+      <c r="L13" s="1">
+        <v>4</v>
+      </c>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1" t="str">
+        <f>IF(O12&lt;O8,"yes","no")</f>
+        <v>no</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>3</v>
+      </c>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1" t="str">
+        <f>IF(T12&lt;T8,"yes","no")</f>
+        <v>no</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="D14">
+        <f>[1]!SignTest(A2:A17,3,2)</f>
+        <v>0.34375000000000011</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1">
+        <v>4</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="J14">
+        <f>[1]!SignTest(G2:G17,3,2)</f>
+        <v>0.3876953125</v>
+      </c>
+      <c r="L14" s="1">
+        <v>5</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="O14">
+        <f>[1]!SignTest(L2:L17,3,2)</f>
+        <v>0.2265625</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>3</v>
+      </c>
+      <c r="R14" s="1"/>
+      <c r="T14">
+        <f>[1]!SignTest(Q2:Q17,3,2)</f>
+        <v>0.34375000000000011</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1">
+        <v>4</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="L15" s="1">
+        <v>5</v>
+      </c>
+      <c r="M15" s="1"/>
+      <c r="Q15" s="1">
+        <v>4</v>
+      </c>
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <f>TINV(D8,D10)</f>
+        <v>2.1314495455597742</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1">
+        <v>4</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16">
+        <f>TINV(J8,J10)</f>
+        <v>2.1314495455597742</v>
+      </c>
+      <c r="L16" s="1">
+        <v>5</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" t="s">
+        <v>14</v>
+      </c>
+      <c r="O16">
+        <f>TINV(O8,O10)</f>
+        <v>2.1447866879178044</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>4</v>
+      </c>
+      <c r="R16" s="1"/>
+      <c r="S16" t="s">
+        <v>14</v>
+      </c>
+      <c r="T16">
+        <f>TINV(T8,T10)</f>
+        <v>2.1314495455597742</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>5</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <f>D7+D16*D5</f>
+        <v>3.5907727468981117</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1">
+        <v>4</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17">
+        <f>J7+J16*J5</f>
+        <v>3.5796537029536424</v>
+      </c>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" t="s">
+        <v>16</v>
+      </c>
+      <c r="O17">
+        <f>O7+O16*O5</f>
+        <v>3.5870631628368406</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>4</v>
+      </c>
+      <c r="R17" s="1"/>
+      <c r="S17" t="s">
+        <v>16</v>
+      </c>
+      <c r="T17">
+        <f>T7+T16*T5</f>
+        <v>3.5101768934334641</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <f>-D16</f>
+        <v>-2.1314495455597742</v>
+      </c>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18">
+        <f>-J16</f>
+        <v>-2.1314495455597742</v>
+      </c>
+      <c r="M18" s="1"/>
+      <c r="N18" t="s">
+        <v>15</v>
+      </c>
+      <c r="O18">
+        <f>-O16</f>
+        <v>-2.1447866879178044</v>
+      </c>
+      <c r="R18" s="1"/>
+      <c r="S18" t="s">
+        <v>15</v>
+      </c>
+      <c r="T18">
+        <f>-T16</f>
+        <v>-2.1314495455597742</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <f>D7+D18*D5</f>
+        <v>2.4092272531018883</v>
+      </c>
+      <c r="I19" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19">
+        <f>J7+J18*J5</f>
+        <v>2.4203462970463576</v>
+      </c>
+      <c r="N19" t="s">
+        <v>17</v>
+      </c>
+      <c r="O19">
+        <f>O7+O18*O5</f>
+        <v>2.4129368371631594</v>
+      </c>
+      <c r="S19" t="s">
+        <v>17</v>
+      </c>
+      <c r="T19">
+        <f>T7+T18*T5</f>
+        <v>2.4898231065665359</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <f>(D17-D3)/D5</f>
+        <v>1.4549681203572276</v>
+      </c>
+      <c r="I20" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20">
+        <f>(J17-J3)/J5</f>
+        <v>1.6718109857828523</v>
+      </c>
+      <c r="N20" t="s">
+        <v>18</v>
+      </c>
+      <c r="O20">
+        <f>(O17-O3)/O5</f>
+        <v>0.19629748612798528</v>
+      </c>
+      <c r="S20" t="s">
+        <v>18</v>
+      </c>
+      <c r="T20">
+        <f>(T17-T3)/T5</f>
+        <v>3.6981484491610552</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <f>(D19-D3)/D5</f>
+        <v>-2.8079309707623192</v>
+      </c>
+      <c r="I21" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21">
+        <f>(J19-J3)/J5</f>
+        <v>-2.5910881053366959</v>
+      </c>
+      <c r="N21" t="s">
+        <v>19</v>
+      </c>
+      <c r="O21">
+        <f>(O19-O3)/O5</f>
+        <v>-4.0932758897076233</v>
+      </c>
+      <c r="S21" t="s">
+        <v>19</v>
+      </c>
+      <c r="T21">
+        <f>(T19-T3)/T5</f>
+        <v>-0.56475064195849412</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <f>[1]!T_DIST(D20,D10,TRUE)</f>
+        <v>0.91685747469378354</v>
+      </c>
+      <c r="I22" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22">
+        <f>[1]!T_DIST(J20,J10,TRUE)</f>
+        <v>0.94235689557653823</v>
+      </c>
+      <c r="N22" t="s">
+        <v>20</v>
+      </c>
+      <c r="O22">
+        <f>[1]!T_DIST(O20,O10,TRUE)</f>
+        <v>0.57640089534202299</v>
+      </c>
+      <c r="S22" t="s">
+        <v>20</v>
+      </c>
+      <c r="T22">
+        <f>[1]!T_DIST(T20,T10,TRUE)</f>
+        <v>0.99892639196560395</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23">
+        <f>[1]!T_DIST(D21,D10,TRUE)</f>
+        <v>6.6230093671768575E-3</v>
+      </c>
+      <c r="I23" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23">
+        <f>[1]!T_DIST(J21,J10,TRUE)</f>
+        <v>1.022930872560901E-2</v>
+      </c>
+      <c r="N23" t="s">
+        <v>21</v>
+      </c>
+      <c r="O23">
+        <f>[1]!T_DIST(O21,O10,TRUE)</f>
+        <v>5.4821922538261791E-4</v>
+      </c>
+      <c r="S23" t="s">
+        <v>21</v>
+      </c>
+      <c r="T23">
+        <f>[1]!T_DIST(T21,T10,TRUE)</f>
+        <v>0.2902958404058838</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24">
+        <f>D22-D23</f>
+        <v>0.91023446532660668</v>
+      </c>
+      <c r="I24" t="s">
+        <v>12</v>
+      </c>
+      <c r="J24">
+        <f>J22-J23</f>
+        <v>0.93212758685092922</v>
+      </c>
+      <c r="N24" t="s">
+        <v>12</v>
+      </c>
+      <c r="O24">
+        <f>O22-O23</f>
+        <v>0.57585267611664037</v>
+      </c>
+      <c r="S24" t="s">
+        <v>12</v>
+      </c>
+      <c r="T24">
+        <f>T22-T23</f>
+        <v>0.70863055155972021</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25">
+        <f>1-D24</f>
+        <v>8.9765534673393321E-2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>13</v>
+      </c>
+      <c r="J25">
+        <f>1-J24</f>
+        <v>6.7872413149070776E-2</v>
+      </c>
+      <c r="N25" t="s">
+        <v>13</v>
+      </c>
+      <c r="O25">
+        <f>1-O24</f>
+        <v>0.42414732388335963</v>
+      </c>
+      <c r="S25" t="s">
+        <v>13</v>
+      </c>
+      <c r="T25">
+        <f>1-T24</f>
+        <v>0.29136944844027979</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="1">
+        <f>TINV(D8*2,D10)</f>
+        <v>1.7530503556925723</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J27" s="1">
+        <f>TINV(J8*2,J10)</f>
+        <v>1.7530503556925723</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O27" s="1">
+        <f>TINV(O8*2,O10)</f>
+        <v>1.7613101357748921</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T27" s="1">
+        <f>TINV(T8*2,T10)</f>
+        <v>1.7530503556925723</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="1">
+        <f>D7+D27*D5</f>
+        <v>3.4858920429248177</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J28" s="1">
+        <f>J7+J27*J5</f>
+        <v>3.4767469782516147</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O28" s="1">
+        <f>O7+O27*O5</f>
+        <v>3.482099364412047</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T28" s="1">
+        <f>T7+T27*T5</f>
+        <v>3.4196044829504899</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="1">
+        <f>(D28-D3)/D5</f>
+        <v>1.0765689304900263</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J29" s="1">
+        <f>(J28-J3)/J5</f>
+        <v>1.293411795915651</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O29" s="1">
+        <f>(O28-O3)/O5</f>
+        <v>-0.18717906601492748</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T29" s="1">
+        <f>(T28-T3)/T5</f>
+        <v>3.3197492592938533</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30">
+        <f>[1]!T_DIST(D29,D10,TRUE)</f>
+        <v>0.85065813539798352</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J30">
+        <f>[1]!T_DIST(J29,J10,TRUE)</f>
+        <v>0.8922834844124633</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O30">
+        <f>[1]!T_DIST(O29,O10,TRUE)</f>
+        <v>0.42710288849756761</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T30">
+        <f>[1]!T_DIST(T29,T10,TRUE)</f>
+        <v>0.99766697008745586</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31">
+        <f>1-D30</f>
+        <v>0.14934186460201648</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J31">
+        <f>1-J30</f>
+        <v>0.1077165155875367</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O31">
+        <f>1-O30</f>
+        <v>0.57289711150243239</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T31">
+        <f>1-T30</f>
+        <v>2.3330299125441378E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="S32" s="1"/>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="C33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <f>(D3-D7)/D4</f>
+        <v>0.16912035630063649</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J33">
+        <f>(J3-J7)/J4</f>
+        <v>0.11490963994423042</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O33">
+        <f>(O3-O7)/O4</f>
+        <v>0.5030977485864635</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T33">
+        <f>(T3-T7)/T4</f>
+        <v>-0.39167472590032015</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="C34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D34">
+        <f>D33*(1-3/(4*D10-1))</f>
+        <v>0.16052101614975667</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J34">
+        <f>J33*(1-3/(4*J10-1))</f>
+        <v>0.10906677689621871</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O34">
+        <f>O33*(1-3/(4*O10-1))</f>
+        <v>0.47565605320902005</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T34">
+        <f>T33*(1-3/(4*T10-1))</f>
+        <v>-0.37175906187149033</v>
+      </c>
+    </row>
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+    </row>
+    <row r="37" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q37" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="V37" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA37" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>3</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1">
+        <f>COUNT(A38:A53)</f>
+        <v>14</v>
+      </c>
+      <c r="G38" s="1">
+        <v>2</v>
+      </c>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J38" s="1">
+        <f>COUNT(G38:G53)</f>
+        <v>14</v>
+      </c>
+      <c r="L38" s="1">
+        <v>3</v>
+      </c>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O38" s="1">
+        <f>COUNT(L38:L53)</f>
+        <v>14</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>3</v>
+      </c>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T38" s="1">
+        <f>COUNT(Q38:Q53)</f>
+        <v>13</v>
+      </c>
+      <c r="V38" s="1">
+        <v>3</v>
+      </c>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="1">
+        <f>COUNT(V38:V53)</f>
+        <v>13</v>
+      </c>
+      <c r="AA38" s="1">
+        <v>2</v>
+      </c>
+      <c r="AB38" s="1"/>
+      <c r="AC38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD38" s="1">
+        <f>COUNT(AA38:AA53)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>3</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1">
+        <f>AVERAGE(A38:A53)</f>
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <f>MEDIAN(A38:A51)</f>
+        <v>4</v>
+      </c>
+      <c r="F39" t="s">
+        <v>35</v>
+      </c>
+      <c r="G39" s="1">
+        <v>2</v>
+      </c>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J39" s="1">
+        <f>AVERAGE(G38:G53)</f>
+        <v>3.5</v>
+      </c>
+      <c r="K39">
+        <f>MEDIAN(G38:G51)</f>
+        <v>4</v>
+      </c>
+      <c r="L39" s="1">
+        <v>3</v>
+      </c>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O39" s="1">
+        <f>AVERAGE(L38:L53)</f>
+        <v>4.2142857142857144</v>
+      </c>
+      <c r="P39">
+        <f>MEDIAN(L38:L51)</f>
+        <v>4</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>3</v>
+      </c>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T39" s="1">
+        <f>AVERAGE(Q38:Q53)</f>
+        <v>4.0769230769230766</v>
+      </c>
+      <c r="U39">
+        <f>MEDIAN(Q38:Q50)</f>
+        <v>4</v>
+      </c>
+      <c r="V39" s="1">
+        <v>3</v>
+      </c>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y39" s="1">
+        <f>AVERAGE(V38:V53)</f>
+        <v>3.6923076923076925</v>
+      </c>
+      <c r="Z39">
+        <f>MEDIAN(V38:V51)</f>
+        <v>4</v>
+      </c>
+      <c r="AA39" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB39" s="1"/>
+      <c r="AC39" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD39" s="1">
+        <f>AVERAGE(AA38:AA53)</f>
+        <v>3.5</v>
+      </c>
+      <c r="AE39">
+        <f>MEDIAN(AA38:AA51)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>3</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="1">
+        <f>_xlfn.STDEV.S(A38:A53)</f>
+        <v>0.67936622048675743</v>
+      </c>
+      <c r="E40">
+        <f>SKEW(A38:A51)</f>
+        <v>-7.9708319716677906E-17</v>
+      </c>
+      <c r="F40" t="s">
+        <v>36</v>
+      </c>
+      <c r="G40" s="1">
+        <v>2</v>
+      </c>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J40" s="1">
+        <f>_xlfn.STDEV.S(G38:G53)</f>
+        <v>1.0190493307301363</v>
+      </c>
+      <c r="K40">
+        <f>SKEW(G38:G51)</f>
+        <v>-0.25441286446211908</v>
+      </c>
+      <c r="L40" s="1">
+        <v>4</v>
+      </c>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O40" s="1">
+        <f>_xlfn.STDEV.S(L38:L53)</f>
+        <v>0.69929320675306816</v>
+      </c>
+      <c r="P40">
+        <f>SKEW(L38:L51)</f>
+        <v>-0.32135175767973356</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>3</v>
+      </c>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T40" s="1">
+        <f>_xlfn.STDEV.S(Q38:Q53)</f>
+        <v>0.86231649850257674</v>
+      </c>
+      <c r="U40">
+        <f>SKEW(Q38:Q50)</f>
+        <v>-0.16358939086282684</v>
+      </c>
+      <c r="V40" s="1">
+        <v>3</v>
+      </c>
+      <c r="W40" s="1"/>
+      <c r="X40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y40" s="1">
+        <f>_xlfn.STDEV.S(V38:V53)</f>
+        <v>0.75106761619881102</v>
+      </c>
+      <c r="Z40">
+        <f>SKEW(V38:V50)</f>
+        <v>0.61070092233746143</v>
+      </c>
+      <c r="AA40" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB40" s="1"/>
+      <c r="AC40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD40" s="1">
+        <f>_xlfn.STDEV.S(AA38:AA53)</f>
+        <v>0.67419986246324204</v>
+      </c>
+      <c r="AE40">
+        <f>SKEW(AA38:AA49)</f>
+        <v>-1.0679325821417758</v>
+      </c>
+    </row>
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>4</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41" s="1">
+        <f>D40/SQRT(D38)</f>
+        <v>0.18156825980064073</v>
+      </c>
+      <c r="E41">
+        <f>_xlfn.MODE.SNGL(A38:A51)</f>
+        <v>4</v>
+      </c>
+      <c r="F41" t="s">
+        <v>37</v>
+      </c>
+      <c r="G41" s="1">
+        <v>3</v>
+      </c>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J41" s="1">
+        <f>J40/SQRT(J38)</f>
+        <v>0.2723523897009611</v>
+      </c>
+      <c r="K41">
+        <f>_xlfn.MODE.SNGL(G38:G51)</f>
+        <v>4</v>
+      </c>
+      <c r="L41" s="1">
+        <v>4</v>
+      </c>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O41" s="1">
+        <f>O40/SQRT(O38)</f>
+        <v>0.18689397089774676</v>
+      </c>
+      <c r="P41">
+        <f>_xlfn.MODE.SNGL(L38:L51)</f>
+        <v>4</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>3</v>
+      </c>
+      <c r="R41" s="1"/>
+      <c r="S41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T41" s="1">
+        <f>T40/SQRT(T38)</f>
+        <v>0.23916356546381592</v>
+      </c>
+      <c r="U41">
+        <f>_xlfn.MODE.SNGL(Q38:Q51)</f>
+        <v>5</v>
+      </c>
+      <c r="V41" s="1">
+        <v>3</v>
+      </c>
+      <c r="W41" s="1"/>
+      <c r="X41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y41" s="1">
+        <f>Y40/SQRT(Y38)</f>
+        <v>0.20830867704194778</v>
+      </c>
+      <c r="Z41">
+        <f>_xlfn.MODE.SNGL(V38:V51)</f>
+        <v>3</v>
+      </c>
+      <c r="AA41" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB41" s="1"/>
+      <c r="AC41" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD41" s="1">
+        <f>AD40/SQRT(AD38)</f>
+        <v>0.19462473604038075</v>
+      </c>
+      <c r="AE41">
+        <f>_xlfn.MODE.SNGL(AA38:AA51)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>4</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="G42" s="1">
+        <v>3</v>
+      </c>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="L42" s="1">
+        <v>4</v>
+      </c>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="Q42" s="1">
+        <v>4</v>
+      </c>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
+      <c r="V42" s="1">
+        <v>3</v>
+      </c>
+      <c r="W42" s="1"/>
+      <c r="X42" s="1"/>
+      <c r="Y42" s="1"/>
+      <c r="AA42" s="1">
+        <v>3</v>
+      </c>
+      <c r="AB42" s="1"/>
+      <c r="AC42" s="1"/>
+      <c r="AD42" s="1"/>
+    </row>
+    <row r="43" spans="1:31" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>4</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="1">
+        <v>3</v>
+      </c>
+      <c r="G43" s="1">
+        <v>3</v>
+      </c>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J43" s="1">
+        <v>3</v>
+      </c>
+      <c r="L43" s="1">
+        <v>4</v>
+      </c>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O43" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>4</v>
+      </c>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T43" s="1">
+        <v>3</v>
+      </c>
+      <c r="V43" s="1">
+        <v>3</v>
+      </c>
+      <c r="W43" s="1"/>
+      <c r="X43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y43" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA43" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB43" s="1"/>
+      <c r="AC43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD43" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>4</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="G44" s="1">
+        <v>4</v>
+      </c>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="L44" s="1">
+        <v>4</v>
+      </c>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O44" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>4</v>
+      </c>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="T44" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="V44" s="1">
+        <v>4</v>
+      </c>
+      <c r="W44" s="1"/>
+      <c r="X44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y44" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="AA44" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB44" s="1"/>
+      <c r="AC44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD44" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>4</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2</v>
+      </c>
+      <c r="G45" s="1">
+        <v>4</v>
+      </c>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J45" s="1">
+        <v>2</v>
+      </c>
+      <c r="L45" s="1">
+        <v>4</v>
+      </c>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O45" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>4</v>
+      </c>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="T45" s="1">
+        <v>2</v>
+      </c>
+      <c r="V45" s="1">
+        <v>4</v>
+      </c>
+      <c r="W45" s="1"/>
+      <c r="X45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y45" s="1">
+        <v>2</v>
+      </c>
+      <c r="AA45" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB45" s="1"/>
+      <c r="AC45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD45" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>4</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="1">
+        <f>D38-1</f>
+        <v>13</v>
+      </c>
+      <c r="G46" s="1">
+        <v>4</v>
+      </c>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J46" s="1">
+        <f>J38-1</f>
+        <v>13</v>
+      </c>
+      <c r="L46" s="1">
+        <v>4</v>
+      </c>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O46" s="1">
+        <f>O38-1</f>
+        <v>13</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>5</v>
+      </c>
+      <c r="R46" s="1"/>
+      <c r="S46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T46" s="1">
+        <f>T38-1</f>
+        <v>12</v>
+      </c>
+      <c r="V46" s="1">
+        <v>4</v>
+      </c>
+      <c r="W46" s="1"/>
+      <c r="X46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y46" s="1">
+        <f>Y38-1</f>
+        <v>12</v>
+      </c>
+      <c r="AA46" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB46" s="1"/>
+      <c r="AC46" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD46" s="1">
+        <f>AD38-1</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>4</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="1">
+        <f>(D39-D43)/D41</f>
+        <v>5.5075705472861021</v>
+      </c>
+      <c r="G47" s="1">
+        <v>4</v>
+      </c>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J47" s="1">
+        <f>(J39-J43)/J41</f>
+        <v>1.8358568490953673</v>
+      </c>
+      <c r="L47" s="1">
+        <v>5</v>
+      </c>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O47" s="1">
+        <f>(O39-O43)/O41</f>
+        <v>6.4971904040182933</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>5</v>
+      </c>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T47" s="1">
+        <f>(T39-T43)/T41</f>
+        <v>4.5028726463187345</v>
+      </c>
+      <c r="V47" s="1">
+        <v>4</v>
+      </c>
+      <c r="W47" s="1"/>
+      <c r="X47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y47" s="1">
+        <f>(Y39-Y43)/Y41</f>
+        <v>3.3234702564419836</v>
+      </c>
+      <c r="AA47" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB47" s="1"/>
+      <c r="AC47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD47" s="1">
+        <f>(AD39-AD43)/AD41</f>
+        <v>2.5690465157330258</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>4</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48">
+        <f>_xlfn.T.DIST.RT(D47,D46)</f>
+        <v>5.042133636310112E-5</v>
+      </c>
+      <c r="G48" s="1">
+        <v>4</v>
+      </c>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J48">
+        <f>_xlfn.T.DIST.2T(J47,J46)</f>
+        <v>8.9349875970482023E-2</v>
+      </c>
+      <c r="L48" s="1">
+        <v>5</v>
+      </c>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O48" s="7">
+        <f>_xlfn.T.DIST.2T(O47,O46)</f>
+        <v>2.0123754997020337E-5</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>5</v>
+      </c>
+      <c r="R48" s="1"/>
+      <c r="S48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="T48">
+        <f>_xlfn.T.DIST.2T(T47,T46)</f>
+        <v>7.2302808206044916E-4</v>
+      </c>
+      <c r="V48" s="1">
+        <v>4</v>
+      </c>
+      <c r="W48" s="1"/>
+      <c r="X48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y48">
+        <f>_xlfn.T.DIST.2T(Y47,Y46)</f>
+        <v>6.0710487499900483E-3</v>
+      </c>
+      <c r="AA48" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB48" s="1"/>
+      <c r="AC48" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD48">
+        <f>_xlfn.T.DIST.2T(AD47,AD46)</f>
+        <v>2.6094682241525793E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>5</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1" t="str">
+        <f>IF(D48&lt;D44,"yes","no")</f>
+        <v>yes</v>
+      </c>
+      <c r="G49" s="1">
+        <v>4</v>
+      </c>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1" t="str">
+        <f>IF(J48&lt;J44,"yes","no")</f>
+        <v>no</v>
+      </c>
+      <c r="L49" s="1">
+        <v>5</v>
+      </c>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1" t="str">
+        <f>IF(O48&lt;O44,"yes","no")</f>
+        <v>yes</v>
+      </c>
+      <c r="Q49" s="1">
+        <v>5</v>
+      </c>
+      <c r="R49" s="1"/>
+      <c r="S49" s="1"/>
+      <c r="T49" s="1" t="str">
+        <f>IF(T48&lt;T44,"yes","no")</f>
+        <v>yes</v>
+      </c>
+      <c r="V49" s="1">
+        <v>5</v>
+      </c>
+      <c r="W49" s="1"/>
+      <c r="X49" s="1"/>
+      <c r="Y49" s="1" t="str">
+        <f>IF(Y48&lt;Y44,"yes","no")</f>
+        <v>yes</v>
+      </c>
+      <c r="AA49" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB49" s="1"/>
+      <c r="AC49" s="1"/>
+      <c r="AD49" s="1" t="str">
+        <f>IF(AD48&lt;AD44,"yes","no")</f>
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>5</v>
+      </c>
+      <c r="B50" s="1"/>
+      <c r="D50" s="8">
+        <f>[1]!SignTest(A38:A51,3)</f>
+        <v>4.8828124999999995E-4</v>
+      </c>
+      <c r="G50" s="1">
+        <v>5</v>
+      </c>
+      <c r="H50" s="1"/>
+      <c r="J50">
+        <f>[1]!SignTest(G38:G51,3)</f>
+        <v>0.11328125</v>
+      </c>
+      <c r="L50" s="1">
+        <v>5</v>
+      </c>
+      <c r="M50" s="1"/>
+      <c r="O50">
+        <f>[1]!SignTest(L38:L51,3)</f>
+        <v>2.4414062500000016E-4</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>5</v>
+      </c>
+      <c r="R50" s="1"/>
+      <c r="T50" s="6">
+        <f>[1]!SignTest(Q38:Q51,3)</f>
+        <v>1.953125E-3</v>
+      </c>
+      <c r="V50" s="1">
+        <v>5</v>
+      </c>
+      <c r="W50" s="1"/>
+      <c r="Y50" s="5">
+        <f>[1]!SignTest(V38:V51,3)</f>
+        <v>7.8125000000000017E-3</v>
+      </c>
+      <c r="AA50" s="1"/>
+      <c r="AB50" s="1"/>
+      <c r="AD50" s="5">
+        <f>[1]!SignTest(AA38:AA51,3)</f>
+        <v>3.5156250000000007E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>5</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="D51">
+        <f>BINOMDIST(0, 11, 0.5, TRUE)</f>
+        <v>4.8828124999999995E-4</v>
+      </c>
+      <c r="G51" s="1">
+        <v>5</v>
+      </c>
+      <c r="H51" s="1"/>
+      <c r="J51">
+        <f>BINOMDIST(3, 11, 0.5, TRUE)</f>
+        <v>0.11328125</v>
+      </c>
+      <c r="L51" s="1">
+        <v>5</v>
+      </c>
+      <c r="M51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1"/>
+      <c r="V51" s="1"/>
+      <c r="W51" s="1"/>
+      <c r="AA51" s="1"/>
+      <c r="AB51" s="1"/>
+    </row>
+    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52">
+        <f>TINV(D44,D46)</f>
+        <v>2.1603686564627926</v>
+      </c>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" t="s">
+        <v>14</v>
+      </c>
+      <c r="J52">
+        <f>TINV(J44,J46)</f>
+        <v>2.1603686564627926</v>
+      </c>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" t="s">
+        <v>14</v>
+      </c>
+      <c r="O52">
+        <f>TINV(O44,O46)</f>
+        <v>2.1603686564627926</v>
+      </c>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1"/>
+      <c r="S52" t="s">
+        <v>14</v>
+      </c>
+      <c r="T52">
+        <f>TINV(T44,T46)</f>
+        <v>2.1788128296672284</v>
+      </c>
+      <c r="V52" s="1"/>
+      <c r="W52" s="1"/>
+      <c r="X52" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y52">
+        <f>TINV(Y44,Y46)</f>
+        <v>2.1788128296672284</v>
+      </c>
+      <c r="AA52" s="1"/>
+      <c r="AB52" s="1"/>
+      <c r="AC52" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD52">
+        <f>TINV(AD44,AD46)</f>
+        <v>2.2009851600916384</v>
+      </c>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53">
+        <f>D43+D52*D41</f>
+        <v>3.3922543774817973</v>
+      </c>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" t="s">
+        <v>16</v>
+      </c>
+      <c r="J53">
+        <f>J43+J52*J41</f>
+        <v>3.5883815662226963</v>
+      </c>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" t="s">
+        <v>16</v>
+      </c>
+      <c r="O53">
+        <f>O43+O52*O41</f>
+        <v>3.4037598768093615</v>
+      </c>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1"/>
+      <c r="S53" t="s">
+        <v>16</v>
+      </c>
+      <c r="T53">
+        <f>T43+T52*T41</f>
+        <v>3.5210926448215201</v>
+      </c>
+      <c r="V53" s="1"/>
+      <c r="W53" s="1"/>
+      <c r="X53" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y53">
+        <f>Y43+Y52*Y41</f>
+        <v>3.4538656180700031</v>
+      </c>
+      <c r="AA53" s="1"/>
+      <c r="AB53" s="1"/>
+      <c r="AC53" t="s">
+        <v>16</v>
+      </c>
+      <c r="AD53">
+        <f>AD43+AD52*AD41</f>
+        <v>3.4283661558116303</v>
+      </c>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54">
+        <f>-D52</f>
+        <v>-2.1603686564627926</v>
+      </c>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" t="s">
+        <v>15</v>
+      </c>
+      <c r="J54">
+        <f>-J52</f>
+        <v>-2.1603686564627926</v>
+      </c>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" t="s">
+        <v>15</v>
+      </c>
+      <c r="O54">
+        <f>-O52</f>
+        <v>-2.1603686564627926</v>
+      </c>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1"/>
+      <c r="S54" t="s">
+        <v>15</v>
+      </c>
+      <c r="T54">
+        <f>-T52</f>
+        <v>-2.1788128296672284</v>
+      </c>
+      <c r="V54" s="1"/>
+      <c r="W54" s="1"/>
+      <c r="X54" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y54">
+        <f>-Y52</f>
+        <v>-2.1788128296672284</v>
+      </c>
+      <c r="AA54" s="1"/>
+      <c r="AB54" s="1"/>
+      <c r="AC54" t="s">
+        <v>15</v>
+      </c>
+      <c r="AD54">
+        <f>-AD52</f>
+        <v>-2.2009851600916384</v>
+      </c>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55">
+        <f>D43+D54*D41</f>
+        <v>2.6077456225182027</v>
+      </c>
+      <c r="I55" t="s">
+        <v>17</v>
+      </c>
+      <c r="J55">
+        <f>J43+J54*J41</f>
+        <v>2.4116184337773037</v>
+      </c>
+      <c r="N55" t="s">
+        <v>17</v>
+      </c>
+      <c r="O55">
+        <f>O43+O54*O41</f>
+        <v>2.5962401231906385</v>
+      </c>
+      <c r="S55" t="s">
+        <v>17</v>
+      </c>
+      <c r="T55">
+        <f>T43+T54*T41</f>
+        <v>2.4789073551784799</v>
+      </c>
+      <c r="X55" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y55">
+        <f>Y43+Y54*Y41</f>
+        <v>2.5461343819299969</v>
+      </c>
+      <c r="AC55" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD55">
+        <f>AD43+AD54*AD41</f>
+        <v>2.5716338441883697</v>
+      </c>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>18</v>
+      </c>
+      <c r="D56">
+        <f>(D53-D39)/D41</f>
+        <v>-3.3472018908233108</v>
+      </c>
+      <c r="I56" t="s">
+        <v>18</v>
+      </c>
+      <c r="J56">
+        <f>(J53-J39)/J41</f>
+        <v>0.32451180736742563</v>
+      </c>
+      <c r="N56" t="s">
+        <v>18</v>
+      </c>
+      <c r="O56">
+        <f>(O53-O39)/O41</f>
+        <v>-4.3368217475554998</v>
+      </c>
+      <c r="S56" t="s">
+        <v>18</v>
+      </c>
+      <c r="T56">
+        <f>(T53-T39)/T41</f>
+        <v>-2.3240598166515065</v>
+      </c>
+      <c r="X56" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y56">
+        <f>(Y53-Y39)/Y41</f>
+        <v>-1.1446574267747547</v>
+      </c>
+      <c r="AC56" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD56">
+        <f>(AD53-AD39)/AD41</f>
+        <v>-0.36806135564138731</v>
+      </c>
+    </row>
+    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57">
+        <f>(D55-D39)/D41</f>
+        <v>-7.6679392037488929</v>
+      </c>
+      <c r="I57" t="s">
+        <v>19</v>
+      </c>
+      <c r="J57">
+        <f>(J55-J39)/J41</f>
+        <v>-3.9962255055581601</v>
+      </c>
+      <c r="N57" t="s">
+        <v>19</v>
+      </c>
+      <c r="O57">
+        <f>(O55-O39)/O41</f>
+        <v>-8.6575590604810859</v>
+      </c>
+      <c r="S57" t="s">
+        <v>19</v>
+      </c>
+      <c r="T57">
+        <f>(T55-T39)/T41</f>
+        <v>-6.6816854759859625</v>
+      </c>
+      <c r="X57" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y57">
+        <f>(Y55-Y39)/Y41</f>
+        <v>-5.5022830861092125</v>
+      </c>
+      <c r="AC57" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD57">
+        <f>(AD55-AD39)/AD41</f>
+        <v>-4.7700316758246641</v>
+      </c>
+    </row>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>20</v>
+      </c>
+      <c r="D58">
+        <f>[1]!T_DIST(D56,D46,TRUE)</f>
+        <v>2.6244361052494836E-3</v>
+      </c>
+      <c r="I58" t="s">
+        <v>20</v>
+      </c>
+      <c r="J58">
+        <f>[1]!T_DIST(J56,J46,TRUE)</f>
+        <v>0.62464344223650536</v>
+      </c>
+      <c r="N58" t="s">
+        <v>20</v>
+      </c>
+      <c r="O58">
+        <f>[1]!T_DIST(O56,O46,TRUE)</f>
+        <v>4.0319945602940166E-4</v>
+      </c>
+      <c r="S58" t="s">
+        <v>20</v>
+      </c>
+      <c r="T58">
+        <f>[1]!T_DIST(T56,T46,TRUE)</f>
+        <v>1.924143314367821E-2</v>
+      </c>
+      <c r="X58" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y58">
+        <f>[1]!T_DIST(Y56,Y46,TRUE)</f>
+        <v>0.13733461179215545</v>
+      </c>
+      <c r="AC58" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD58">
+        <f>[1]!T_DIST(AD56,AD46,TRUE)</f>
+        <v>0.35990600742088347</v>
+      </c>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59">
+        <f>[1]!T_DIST(D57,D46,TRUE)</f>
+        <v>1.7729238882546738E-6</v>
+      </c>
+      <c r="I59" t="s">
+        <v>21</v>
+      </c>
+      <c r="J59">
+        <f>[1]!T_DIST(J57,J46,TRUE)</f>
+        <v>7.614326298340246E-4</v>
+      </c>
+      <c r="N59" t="s">
+        <v>21</v>
+      </c>
+      <c r="O59">
+        <f>[1]!T_DIST(O57,O46,TRUE)</f>
+        <v>4.6603147807466883E-7</v>
+      </c>
+      <c r="S59" t="s">
+        <v>21</v>
+      </c>
+      <c r="T59">
+        <f>[1]!T_DIST(T57,T46,TRUE)</f>
+        <v>1.1273998069993851E-5</v>
+      </c>
+      <c r="X59" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y59">
+        <f>[1]!T_DIST(Y57,Y46,TRUE)</f>
+        <v>6.7878982039637492E-5</v>
+      </c>
+      <c r="AC59" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD59">
+        <f>[1]!T_DIST(AD57,AD46,TRUE)</f>
+        <v>2.9032531611394852E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60">
+        <f>D58-D59</f>
+        <v>2.6226631813612289E-3</v>
+      </c>
+      <c r="I60" t="s">
+        <v>12</v>
+      </c>
+      <c r="J60">
+        <f>J58-J59</f>
+        <v>0.62388200960667128</v>
+      </c>
+      <c r="N60" t="s">
+        <v>12</v>
+      </c>
+      <c r="O60">
+        <f>O58-O59</f>
+        <v>4.0273342455132699E-4</v>
+      </c>
+      <c r="S60" t="s">
+        <v>12</v>
+      </c>
+      <c r="T60">
+        <f>T58-T59</f>
+        <v>1.9230159145608217E-2</v>
+      </c>
+      <c r="X60" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y60">
+        <f>Y58-Y59</f>
+        <v>0.13726673281011581</v>
+      </c>
+      <c r="AC60" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD60">
+        <f>AD58-AD59</f>
+        <v>0.35961568210476952</v>
+      </c>
+    </row>
+    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>13</v>
+      </c>
+      <c r="D61">
+        <f>1-D60</f>
+        <v>0.99737733681863872</v>
+      </c>
+      <c r="I61" t="s">
+        <v>13</v>
+      </c>
+      <c r="J61">
+        <f>1-J60</f>
+        <v>0.37611799039332872</v>
+      </c>
+      <c r="N61" t="s">
+        <v>13</v>
+      </c>
+      <c r="O61">
+        <f>1-O60</f>
+        <v>0.99959726657544867</v>
+      </c>
+      <c r="S61" t="s">
+        <v>13</v>
+      </c>
+      <c r="T61">
+        <f>1-T60</f>
+        <v>0.98076984085439178</v>
+      </c>
+      <c r="X61" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y61">
+        <f>1-Y60</f>
+        <v>0.86273326718988419</v>
+      </c>
+      <c r="AC61" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD61">
+        <f>1-AD60</f>
+        <v>0.64038431789523043</v>
+      </c>
+    </row>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="S62" s="1"/>
+      <c r="T62" s="1"/>
+      <c r="X62" s="1"/>
+      <c r="Y62" s="1"/>
+      <c r="AC62" s="1"/>
+      <c r="AD62" s="1"/>
+    </row>
+    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D63" s="1">
+        <f>TINV(D44*2,D46)</f>
+        <v>1.7709333959868729</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J63" s="1">
+        <f>TINV(J44*2,J46)</f>
+        <v>1.7709333959868729</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O63" s="1">
+        <f>TINV(O44*2,O46)</f>
+        <v>1.7709333959868729</v>
+      </c>
+      <c r="S63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T63" s="1">
+        <f>TINV(T44*2,T46)</f>
+        <v>1.7822875556493194</v>
+      </c>
+      <c r="X63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y63" s="1">
+        <f>TINV(Y44*2,Y46)</f>
+        <v>1.7822875556493194</v>
+      </c>
+      <c r="AC63" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD63" s="1">
+        <f>TINV(AD44*2,AD46)</f>
+        <v>1.7958848187040437</v>
+      </c>
+    </row>
+    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="C64" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D64" s="1">
+        <f>D43+D63*D41</f>
+        <v>3.3215452949321755</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J64" s="1">
+        <f>J43+J63*J41</f>
+        <v>3.4823179423982631</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O64" s="1">
+        <f>O43+O63*O41</f>
+        <v>3.3309767745714183</v>
+      </c>
+      <c r="S64" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T64" s="1">
+        <f>T43+T63*T41</f>
+        <v>3.4262582464908804</v>
+      </c>
+      <c r="X64" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y64" s="1">
+        <f>Y43+Y63*Y41</f>
+        <v>3.3712659628256367</v>
+      </c>
+      <c r="AC64" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD64" s="1">
+        <f>AD43+AD63*AD41</f>
+        <v>3.3495236087992017</v>
+      </c>
+    </row>
+    <row r="65" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="C65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" s="1">
+        <f>(D64-D39)/D41</f>
+        <v>-3.7366371512992287</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J65" s="1">
+        <f>(J64-J39)/J41</f>
+        <v>-6.4923453108495024E-2</v>
+      </c>
+      <c r="N65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O65" s="1">
+        <f>(O64-O39)/O41</f>
+        <v>-4.7262570080314212</v>
+      </c>
+      <c r="S65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T65" s="1">
+        <f>(T64-T39)/T41</f>
+        <v>-2.7205850906694153</v>
+      </c>
+      <c r="X65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y65" s="1">
+        <f>(Y64-Y39)/Y41</f>
+        <v>-1.5411827007926635</v>
+      </c>
+      <c r="AC65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AD65" s="1">
+        <f>(AD64-AD39)/AD41</f>
+        <v>-0.77316169702898097</v>
+      </c>
+    </row>
+    <row r="66" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="C66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66">
+        <f>[1]!T_DIST(D65,D46,TRUE)</f>
+        <v>1.2450096195885108E-3</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J66">
+        <f>[1]!T_DIST(J65,J46,TRUE)</f>
+        <v>0.47461135019513728</v>
+      </c>
+      <c r="N66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O66">
+        <f>[1]!T_DIST(O65,O46,TRUE)</f>
+        <v>1.9800393332164434E-4</v>
+      </c>
+      <c r="S66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T66">
+        <f>[1]!T_DIST(T65,T46,TRUE)</f>
+        <v>9.293831013380216E-3</v>
+      </c>
+      <c r="X66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y66">
+        <f>[1]!T_DIST(Y65,Y46,TRUE)</f>
+        <v>7.4609410822665478E-2</v>
+      </c>
+      <c r="AC66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD66">
+        <f>[1]!T_DIST(AD65,AD46,TRUE)</f>
+        <v>0.22786010564673542</v>
+      </c>
+    </row>
+    <row r="67" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="C67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D67">
+        <f>1-D66</f>
+        <v>0.99875499038041149</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J67">
+        <f>1-J66</f>
+        <v>0.52538864980486277</v>
+      </c>
+      <c r="N67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O67">
+        <f>1-O66</f>
+        <v>0.99980199606667841</v>
+      </c>
+      <c r="S67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T67">
+        <f>1-T66</f>
+        <v>0.99070616898661978</v>
+      </c>
+      <c r="X67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y67">
+        <f>1-Y66</f>
+        <v>0.92539058917733452</v>
+      </c>
+      <c r="AC67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD67">
+        <f>1-AD66</f>
+        <v>0.77213989435326458</v>
+      </c>
+    </row>
+    <row r="68" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="C68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="S68" s="1"/>
+      <c r="X68" s="1"/>
+      <c r="AC68" s="1"/>
+    </row>
+    <row r="69" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="C69" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D69">
+        <f>(D39-D43)/D40</f>
+        <v>1.4719601443879746</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J69">
+        <f>(J39-J43)/J40</f>
+        <v>0.49065338146265813</v>
+      </c>
+      <c r="N69" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O69">
+        <f>(O39-O43)/O40</f>
+        <v>1.7364471763194154</v>
+      </c>
+      <c r="S69" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T69">
+        <f>(T39-T43)/T40</f>
+        <v>1.2488721702451093</v>
+      </c>
+      <c r="X69" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y69">
+        <f>(Y39-Y43)/Y40</f>
+        <v>0.92176480169854047</v>
+      </c>
+      <c r="AC69" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD69">
+        <f>(AD39-AD43)/AD40</f>
+        <v>0.74161984870956632</v>
+      </c>
+    </row>
+    <row r="70" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="C70" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D70">
+        <f>D69*(1-3/(4*D46-1))</f>
+        <v>1.3853742535416231</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J70">
+        <f>J69*(1-3/(4*J46-1))</f>
+        <v>0.46179141784720767</v>
+      </c>
+      <c r="N70" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O70">
+        <f>O69*(1-3/(4*O46-1))</f>
+        <v>1.6343032247712144</v>
+      </c>
+      <c r="S70" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="T70">
+        <f>T69*(1-3/(4*T46-1))</f>
+        <v>1.1691569253358471</v>
+      </c>
+      <c r="X70" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y70">
+        <f>Y69*(1-3/(4*Y46-1))</f>
+        <v>0.86292875052629325</v>
+      </c>
+      <c r="AC70" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD70">
+        <f>AD69*(1-3/(4*AD46-1))</f>
+        <v>0.68987892903215475</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,6 +3570,7 @@
     <col min="12" max="12" width="13" customWidth="1"/>
     <col min="14" max="14" width="10.85546875" customWidth="1"/>
     <col min="19" max="19" width="15" customWidth="1"/>
+    <col min="24" max="24" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -1034,19 +4102,35 @@
         <v>4</v>
       </c>
       <c r="B13" s="1"/>
+      <c r="D13">
+        <f>[1]!SignTest(A1:A16,3,2)</f>
+        <v>0.34375000000000011</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1">
         <v>4</v>
       </c>
       <c r="G13" s="1"/>
+      <c r="I13">
+        <f>[1]!SignTest(F1:F16,3,2)</f>
+        <v>0.3876953125</v>
+      </c>
       <c r="K13" s="1">
         <v>5</v>
       </c>
       <c r="L13" s="1"/>
+      <c r="N13">
+        <f>[1]!SignTest(K1:K16,3,2)</f>
+        <v>0.2265625</v>
+      </c>
       <c r="P13" s="1">
         <v>3</v>
       </c>
       <c r="Q13" s="1"/>
+      <c r="S13">
+        <f>[1]!SignTest(P1:P16,3,2)</f>
+        <v>0.34375000000000011</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -2461,24 +5545,48 @@
         <v>5</v>
       </c>
       <c r="B48" s="1"/>
+      <c r="D48">
+        <f>[1]!SignTest(A36:A49,3)</f>
+        <v>4.8828124999999995E-4</v>
+      </c>
       <c r="F48" s="1">
         <v>5</v>
       </c>
       <c r="G48" s="1"/>
+      <c r="I48">
+        <f>[1]!SignTest(F36:F49,3)</f>
+        <v>0.11328125</v>
+      </c>
       <c r="K48" s="1">
         <v>5</v>
       </c>
       <c r="L48" s="1"/>
+      <c r="N48">
+        <f>[1]!SignTest(K36:K49,3)</f>
+        <v>2.4414062500000016E-4</v>
+      </c>
       <c r="P48" s="1">
         <v>5</v>
       </c>
       <c r="Q48" s="1"/>
+      <c r="S48">
+        <f>[1]!SignTest(P36:P49,3)</f>
+        <v>1.953125E-3</v>
+      </c>
       <c r="U48" s="1">
         <v>5</v>
       </c>
       <c r="V48" s="1"/>
+      <c r="X48">
+        <f>[1]!SignTest(U36:U49,3)</f>
+        <v>7.8125000000000017E-3</v>
+      </c>
       <c r="Z48" s="1"/>
       <c r="AA48" s="1"/>
+      <c r="AC48">
+        <f>[1]!SignTest(Z36:Z49,3)</f>
+        <v>3.5156250000000007E-2</v>
+      </c>
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
@@ -3307,18 +6415,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3333,4 +6429,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>